<commit_message>
Making changes to excel files and adding additional calculations
</commit_message>
<xml_diff>
--- a/Procurement/Delivery_Data.xlsx
+++ b/Procurement/Delivery_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\ISYS40251_Deriving-Value-Data-Analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\ISYS40251_Deriving-Value-Data-Analytics\Procurement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62946ABC-454E-452F-847C-393C2D8BD70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7C288F-4088-4F47-BB6F-51837CA65BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1097"/>
+  <dimension ref="A1:F1097"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1097"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,7 +423,7 @@
     <col min="4" max="4" width="28.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44562</v>
       </c>
@@ -451,8 +451,9 @@
         <v>88.647711691201209</v>
       </c>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44563</v>
       </c>
@@ -466,7 +467,7 @@
         <v>92.469400456399981</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44564</v>
       </c>
@@ -480,7 +481,7 @@
         <v>96.261090859068716</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44565</v>
       </c>
@@ -494,7 +495,7 @@
         <v>93.335182744989254</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44566</v>
       </c>
@@ -508,7 +509,7 @@
         <v>87.547475891903019</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44567</v>
       </c>
@@ -522,7 +523,7 @@
         <v>92.969788312666992</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>44568</v>
       </c>
@@ -536,7 +537,7 @@
         <v>95.050665773385816</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>44569</v>
       </c>
@@ -550,7 +551,7 @@
         <v>88.501539791452814</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>44570</v>
       </c>
@@ -564,7 +565,7 @@
         <v>93.368901388257029</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>44571</v>
       </c>
@@ -578,7 +579,7 @@
         <v>89.749177846218103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>44572</v>
       </c>
@@ -592,7 +593,7 @@
         <v>90.059254742367798</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>44573</v>
       </c>
@@ -606,7 +607,7 @@
         <v>82.622416905462217</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>44574</v>
       </c>
@@ -620,7 +621,7 @@
         <v>85.81498586359973</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>44575</v>
       </c>
@@ -634,7 +635,7 @@
         <v>87.86045677081998</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>44576</v>
       </c>

</xml_diff>